<commit_message>
version 1.3 - Fixed warnings and errors
</commit_message>
<xml_diff>
--- a/Project Ontwerp BOM.xlsx
+++ b/Project Ontwerp BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PatrickKenis\Desktop\School documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AltiumProjects\2023\SoldeerStation2223\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622F0530-8EFB-44AD-9364-5D8EE4043655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA1161C-931C-49A3-B263-06D131C5527E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-14160" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{F3C9ADDF-87B1-4935-BA06-AA4BBB1134FD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{F3C9ADDF-87B1-4935-BA06-AA4BBB1134FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="271">
   <si>
     <t>weerstanden</t>
   </si>
@@ -837,6 +837,21 @@
   </si>
   <si>
     <t>R6,R7,R19,R23,R24,R25</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/nl/p/sks-hirschmann-agf-20-fijn-krokodilklem-zilver-klembereik-max-10-mm-lengte-49-mm-1-stuk-s-735175.html</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>have</t>
+  </si>
+  <si>
+    <t>krokodillenklem</t>
+  </si>
+  <si>
+    <t>Soldeerbout</t>
   </si>
 </sst>
 </file>
@@ -1102,7 +1117,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1290,6 +1305,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="15" fillId="8" borderId="2" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3018,8 +3039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F4DDA4E-0942-45CA-A400-627CF5A7DA99}">
   <dimension ref="A1:AE60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4353,8 +4374,8 @@
       <c r="J36" t="s">
         <v>245</v>
       </c>
-      <c r="K36" s="69" t="s">
-        <v>250</v>
+      <c r="K36" s="74" t="s">
+        <v>249</v>
       </c>
       <c r="P36" s="41">
         <v>6.7560970526315813</v>
@@ -4387,8 +4408,8 @@
       <c r="J37" t="s">
         <v>246</v>
       </c>
-      <c r="K37" s="69" t="s">
-        <v>250</v>
+      <c r="K37" s="74" t="s">
+        <v>249</v>
       </c>
       <c r="Q37" s="41"/>
     </row>
@@ -4415,8 +4436,8 @@
       <c r="J38" t="s">
         <v>246</v>
       </c>
-      <c r="K38" s="69" t="s">
-        <v>250</v>
+      <c r="K38" s="74" t="s">
+        <v>249</v>
       </c>
       <c r="P38" s="41">
         <v>128.36584400000004</v>
@@ -4450,8 +4471,8 @@
       <c r="J39" t="s">
         <v>246</v>
       </c>
-      <c r="K39" s="69" t="s">
-        <v>250</v>
+      <c r="K39" s="74" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
@@ -4477,8 +4498,8 @@
       <c r="J40" t="s">
         <v>246</v>
       </c>
-      <c r="K40" s="69" t="s">
-        <v>250</v>
+      <c r="K40" s="74" t="s">
+        <v>249</v>
       </c>
       <c r="Q40" s="41"/>
     </row>
@@ -4505,8 +4526,8 @@
       <c r="J41" t="s">
         <v>246</v>
       </c>
-      <c r="K41" s="69" t="s">
-        <v>250</v>
+      <c r="K41" s="74" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
@@ -4772,19 +4793,35 @@
       <c r="E54" s="1"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
+      <c r="A55" s="1" t="s">
+        <v>267</v>
+      </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="C56" s="1"/>
+      <c r="A56" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C56" s="73" t="s">
+        <v>266</v>
+      </c>
       <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
+      <c r="E56" s="1">
+        <v>2</v>
+      </c>
+      <c r="G56">
+        <v>1.29</v>
+      </c>
+      <c r="J56" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
+      <c r="A57" s="1" t="s">
+        <v>270</v>
+      </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -4842,9 +4879,10 @@
     <hyperlink ref="D34" r:id="rId32" display="https://www.lcsc.com/product-detail/span-style-background-color-ff0-Led-span-span-style-background-color-ff0-Segment-span-Display_Shenzhen-Zhihao-Elec-FJ3661BH_C68298.html" xr:uid="{5E648631-E01B-4ED4-9519-CCAAFDFF66F9}"/>
     <hyperlink ref="C45" r:id="rId33" xr:uid="{9FFCAB6B-B425-4662-9851-FFC8B94CAE45}"/>
     <hyperlink ref="C46" r:id="rId34" xr:uid="{0F6E49AF-4BAA-49B1-87E6-98CA56E983C2}"/>
+    <hyperlink ref="C56" r:id="rId35" xr:uid="{A9AEA7C2-91AB-4B6E-A63D-CE8D39625EB5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId35"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId36"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Version 1.5 - added PCB
fixed shematic designs
added logic PCB and display PCB
</commit_message>
<xml_diff>
--- a/Project Ontwerp BOM.xlsx
+++ b/Project Ontwerp BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AltiumProjects\2023\SoldeerStation2223\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA1161C-931C-49A3-B263-06D131C5527E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3746160A-2708-4038-8D0A-C05675104B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{F3C9ADDF-87B1-4935-BA06-AA4BBB1134FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F3C9ADDF-87B1-4935-BA06-AA4BBB1134FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="276">
   <si>
     <t>weerstanden</t>
   </si>
@@ -776,9 +776,6 @@
     <t>Group buy</t>
   </si>
   <si>
-    <t>Ordered</t>
-  </si>
-  <si>
     <t>Not ordered</t>
   </si>
   <si>
@@ -852,6 +849,24 @@
   </si>
   <si>
     <t>Soldeerbout</t>
+  </si>
+  <si>
+    <t>Have</t>
+  </si>
+  <si>
+    <t>K4,K7,K10,K14,K15</t>
+  </si>
+  <si>
+    <t>https://benl.rs-online.com/web/p/pcb-headers/2518632</t>
+  </si>
+  <si>
+    <t>voedings jumpers</t>
+  </si>
+  <si>
+    <t>https://benl.rs-online.com/web/p/jumpers-shunts/6742393</t>
+  </si>
+  <si>
+    <t>Optional</t>
   </si>
 </sst>
 </file>
@@ -1117,7 +1132,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1277,9 +1292,6 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="2" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1312,6 +1324,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3037,10 +3073,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F4DDA4E-0942-45CA-A400-627CF5A7DA99}">
-  <dimension ref="A1:AE60"/>
+  <dimension ref="A1:AE61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3050,6 +3086,7 @@
     <col min="3" max="3" width="126" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" customWidth="1"/>
     <col min="11" max="11" width="9.7109375" customWidth="1"/>
     <col min="12" max="12" width="10.85546875" customWidth="1"/>
@@ -3085,10 +3122,10 @@
         <v>235</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3141,8 +3178,8 @@
       <c r="J3" t="s">
         <v>244</v>
       </c>
-      <c r="K3" s="64" t="s">
-        <v>248</v>
+      <c r="K3" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="N3" s="57"/>
       <c r="Q3" s="41"/>
@@ -3181,8 +3218,8 @@
       <c r="J4" t="s">
         <v>244</v>
       </c>
-      <c r="K4" s="64" t="s">
-        <v>248</v>
+      <c r="K4" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="N4" s="57"/>
       <c r="Q4" s="41"/>
@@ -3221,8 +3258,8 @@
       <c r="J5" t="s">
         <v>244</v>
       </c>
-      <c r="K5" s="64" t="s">
-        <v>248</v>
+      <c r="K5" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="N5" s="57"/>
       <c r="Q5" s="41"/>
@@ -3261,25 +3298,25 @@
       <c r="J6" t="s">
         <v>244</v>
       </c>
-      <c r="K6" s="64" t="s">
-        <v>248</v>
+      <c r="K6" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="N6" s="57"/>
       <c r="Q6" s="41"/>
       <c r="X6" s="62" t="s">
+        <v>250</v>
+      </c>
+      <c r="Y6" s="62" t="s">
         <v>251</v>
       </c>
-      <c r="Y6" s="62" t="s">
+      <c r="Z6" s="62" t="s">
         <v>252</v>
       </c>
-      <c r="Z6" s="62" t="s">
+      <c r="AA6" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="AA6" s="62" t="s">
+      <c r="AB6" s="62" t="s">
         <v>254</v>
-      </c>
-      <c r="AB6" s="62" t="s">
-        <v>255</v>
       </c>
       <c r="AD6" s="62" t="s">
         <v>236</v>
@@ -3293,7 +3330,7 @@
         <v>128</v>
       </c>
       <c r="B7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C7" s="31" t="s">
         <v>204</v>
@@ -3322,28 +3359,28 @@
       <c r="J7" t="s">
         <v>244</v>
       </c>
-      <c r="K7" s="64" t="s">
-        <v>248</v>
+      <c r="K7" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="N7" s="57"/>
       <c r="Q7" s="41"/>
-      <c r="X7" s="71">
+      <c r="X7" s="70">
         <f>SUM(I3:I10,I12,I15:I19,I21:I27,I32:I34,I45:I46)</f>
         <v>8.4549240000000001</v>
       </c>
-      <c r="Y7" s="71">
+      <c r="Y7" s="70">
         <f>SUM(I28:I31,I13)</f>
         <v>17.09</v>
       </c>
-      <c r="Z7" s="71">
+      <c r="Z7" s="70">
         <f>SUM(I36,I42,I48:I49)</f>
         <v>5.3800000000000008</v>
       </c>
-      <c r="AA7" s="71">
+      <c r="AA7" s="70">
         <f>SUM(I44)</f>
         <v>49.03</v>
       </c>
-      <c r="AB7" s="71">
+      <c r="AB7" s="70">
         <f>SUM(I47)</f>
         <v>9.99</v>
       </c>
@@ -3388,30 +3425,30 @@
       <c r="J8" t="s">
         <v>244</v>
       </c>
-      <c r="K8" s="64" t="s">
-        <v>248</v>
+      <c r="K8" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="N8" s="57"/>
       <c r="Q8" s="41"/>
-      <c r="X8" s="72">
+      <c r="X8" s="71">
         <f>X7/$I$51</f>
-        <v>9.4001124510372597E-2</v>
-      </c>
-      <c r="Y8" s="72">
+        <v>8.2082716744686882E-2</v>
+      </c>
+      <c r="Y8" s="71">
         <f t="shared" ref="Y8:AB8" si="3">Y7/$I$51</f>
-        <v>0.1900051636043408</v>
-      </c>
-      <c r="Z8" s="72">
+        <v>0.16591439842235114</v>
+      </c>
+      <c r="Z8" s="71">
         <f t="shared" si="3"/>
-        <v>5.9814381520851591E-2</v>
-      </c>
-      <c r="AA8" s="72">
+        <v>5.2230512785971288E-2</v>
+      </c>
+      <c r="AA8" s="71">
         <f t="shared" si="3"/>
-        <v>0.54511136170396901</v>
-      </c>
-      <c r="AB8" s="72">
+        <v>0.47599666206248548</v>
+      </c>
+      <c r="AB8" s="71">
         <f t="shared" si="3"/>
-        <v>0.11106796866046605</v>
+        <v>9.6985654782872327E-2</v>
       </c>
     </row>
     <row r="9" spans="1:31" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3448,8 +3485,8 @@
       <c r="J9" t="s">
         <v>244</v>
       </c>
-      <c r="K9" s="64" t="s">
-        <v>248</v>
+      <c r="K9" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="N9" s="57"/>
       <c r="Q9" s="41"/>
@@ -3492,8 +3529,8 @@
       <c r="J10" t="s">
         <v>244</v>
       </c>
-      <c r="K10" s="64" t="s">
-        <v>248</v>
+      <c r="K10" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="N10" s="57"/>
       <c r="Q10" s="41"/>
@@ -3511,7 +3548,7 @@
       <c r="H11" s="42"/>
       <c r="I11" s="42"/>
       <c r="J11" s="17"/>
-      <c r="K11" s="65"/>
+      <c r="K11" s="64"/>
       <c r="L11" s="17"/>
     </row>
     <row r="12" spans="1:31" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3548,8 +3585,8 @@
       <c r="J12" t="s">
         <v>244</v>
       </c>
-      <c r="K12" s="64" t="s">
-        <v>248</v>
+      <c r="K12" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="N12" s="57"/>
       <c r="Q12" s="41"/>
@@ -3588,8 +3625,8 @@
       <c r="J13" t="s">
         <v>244</v>
       </c>
-      <c r="K13" s="64" t="s">
-        <v>248</v>
+      <c r="K13" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="Q13" s="41"/>
     </row>
@@ -3606,7 +3643,7 @@
       <c r="H14" s="43"/>
       <c r="I14" s="43"/>
       <c r="J14" s="21"/>
-      <c r="K14" s="66"/>
+      <c r="K14" s="65"/>
       <c r="L14" s="21"/>
     </row>
     <row r="15" spans="1:31" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3643,8 +3680,8 @@
       <c r="J15" t="s">
         <v>244</v>
       </c>
-      <c r="K15" s="64" t="s">
-        <v>248</v>
+      <c r="K15" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="N15" s="57"/>
       <c r="Q15" s="41"/>
@@ -3683,8 +3720,8 @@
       <c r="J16" t="s">
         <v>244</v>
       </c>
-      <c r="K16" s="64" t="s">
-        <v>248</v>
+      <c r="K16" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="N16" s="57"/>
       <c r="Q16" s="41"/>
@@ -3694,7 +3731,7 @@
         <v>146</v>
       </c>
       <c r="B17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="15">
@@ -3716,8 +3753,8 @@
       <c r="J17" t="s">
         <v>244</v>
       </c>
-      <c r="K17" s="67" t="s">
-        <v>249</v>
+      <c r="K17" s="66" t="s">
+        <v>248</v>
       </c>
       <c r="N17" s="57"/>
     </row>
@@ -3726,7 +3763,7 @@
         <v>147</v>
       </c>
       <c r="B18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C18" s="31" t="s">
         <v>211</v>
@@ -3755,8 +3792,8 @@
       <c r="J18" t="s">
         <v>244</v>
       </c>
-      <c r="K18" s="64" t="s">
-        <v>248</v>
+      <c r="K18" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="N18" s="57"/>
       <c r="Q18" s="41"/>
@@ -3766,7 +3803,7 @@
         <v>150</v>
       </c>
       <c r="B19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C19" s="31" t="s">
         <v>212</v>
@@ -3795,8 +3832,8 @@
       <c r="J19" t="s">
         <v>244</v>
       </c>
-      <c r="K19" s="64" t="s">
-        <v>248</v>
+      <c r="K19" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="N19" s="57"/>
       <c r="Q19" s="41"/>
@@ -3814,7 +3851,7 @@
       <c r="H20" s="44"/>
       <c r="I20" s="44"/>
       <c r="J20" s="22"/>
-      <c r="K20" s="68"/>
+      <c r="K20" s="67"/>
       <c r="L20" s="22"/>
     </row>
     <row r="21" spans="1:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3843,8 +3880,8 @@
       <c r="J21" t="s">
         <v>244</v>
       </c>
-      <c r="K21" s="69" t="s">
-        <v>250</v>
+      <c r="K21" s="68" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:25" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3878,8 +3915,8 @@
       <c r="J22" t="s">
         <v>244</v>
       </c>
-      <c r="K22" s="64" t="s">
-        <v>248</v>
+      <c r="K22" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="N22" s="57"/>
       <c r="Q22" s="41"/>
@@ -3915,8 +3952,8 @@
       <c r="J23" t="s">
         <v>244</v>
       </c>
-      <c r="K23" s="64" t="s">
-        <v>248</v>
+      <c r="K23" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="N23" s="57"/>
       <c r="Q23" s="41"/>
@@ -3952,8 +3989,8 @@
       <c r="J24" t="s">
         <v>244</v>
       </c>
-      <c r="K24" s="64" t="s">
-        <v>248</v>
+      <c r="K24" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="N24" s="57"/>
       <c r="Q24" s="41"/>
@@ -3989,8 +4026,8 @@
       <c r="J25" t="s">
         <v>244</v>
       </c>
-      <c r="K25" s="64" t="s">
-        <v>248</v>
+      <c r="K25" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="N25" s="57"/>
       <c r="Q25" s="41"/>
@@ -4026,8 +4063,8 @@
       <c r="J26" t="s">
         <v>244</v>
       </c>
-      <c r="K26" s="64" t="s">
-        <v>248</v>
+      <c r="K26" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="N26" s="57"/>
       <c r="Q26" s="41"/>
@@ -4063,8 +4100,8 @@
       <c r="J27" t="s">
         <v>244</v>
       </c>
-      <c r="K27" s="64" t="s">
-        <v>248</v>
+      <c r="K27" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="N27" s="57"/>
       <c r="Q27" s="41"/>
@@ -4100,8 +4137,8 @@
       <c r="J28" t="s">
         <v>244</v>
       </c>
-      <c r="K28" s="64" t="s">
-        <v>248</v>
+      <c r="K28" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="Q28" s="41"/>
     </row>
@@ -4136,8 +4173,8 @@
       <c r="J29" t="s">
         <v>244</v>
       </c>
-      <c r="K29" s="64" t="s">
-        <v>248</v>
+      <c r="K29" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="Q29" s="41"/>
     </row>
@@ -4172,8 +4209,8 @@
       <c r="J30" t="s">
         <v>244</v>
       </c>
-      <c r="K30" s="64" t="s">
-        <v>248</v>
+      <c r="K30" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="Q30" s="41"/>
     </row>
@@ -4208,8 +4245,8 @@
       <c r="J31" t="s">
         <v>244</v>
       </c>
-      <c r="K31" s="64" t="s">
-        <v>248</v>
+      <c r="K31" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="Q31" s="41"/>
       <c r="R31" s="41"/>
@@ -4245,8 +4282,8 @@
       <c r="J32" t="s">
         <v>244</v>
       </c>
-      <c r="K32" s="64" t="s">
-        <v>248</v>
+      <c r="K32" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="N32" s="57"/>
       <c r="Q32" s="41"/>
@@ -4283,8 +4320,8 @@
       <c r="J33" t="s">
         <v>244</v>
       </c>
-      <c r="K33" s="64" t="s">
-        <v>248</v>
+      <c r="K33" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="N33" s="57"/>
       <c r="Q33" s="41"/>
@@ -4297,7 +4334,7 @@
         <v>197</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E34" s="34">
         <v>1</v>
@@ -4318,10 +4355,10 @@
         <v>2.2559999999999998</v>
       </c>
       <c r="J34" t="s">
-        <v>246</v>
-      </c>
-      <c r="K34" s="64" t="s">
-        <v>248</v>
+        <v>245</v>
+      </c>
+      <c r="K34" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="V34" s="41"/>
     </row>
@@ -4338,7 +4375,7 @@
       <c r="H35" s="45"/>
       <c r="I35" s="45"/>
       <c r="J35" s="36"/>
-      <c r="K35" s="70"/>
+      <c r="K35" s="69"/>
       <c r="L35" s="36"/>
       <c r="S35" s="41"/>
       <c r="V35" s="41"/>
@@ -4372,16 +4409,16 @@
         <v>1.6</v>
       </c>
       <c r="J36" t="s">
-        <v>245</v>
-      </c>
-      <c r="K36" s="74" t="s">
-        <v>249</v>
+        <v>270</v>
+      </c>
+      <c r="K36" s="73" t="s">
+        <v>248</v>
       </c>
       <c r="P36" s="41">
         <v>6.7560970526315813</v>
       </c>
       <c r="Q36" s="41" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="V36" s="41"/>
     </row>
@@ -4390,26 +4427,34 @@
         <v>219</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
-      </c>
-      <c r="E37" s="32">
-        <v>3</v>
-      </c>
-      <c r="F37" s="48"/>
-      <c r="G37" s="57"/>
-      <c r="H37" s="48">
+        <v>271</v>
+      </c>
+      <c r="C37" s="81" t="s">
+        <v>272</v>
+      </c>
+      <c r="E37" s="76">
+        <v>1</v>
+      </c>
+      <c r="F37" s="77">
+        <f t="shared" ref="F37:F41" si="7">G37/$AE$7</f>
+        <v>13.893617021276597</v>
+      </c>
+      <c r="G37" s="80">
+        <v>13.06</v>
+      </c>
+      <c r="H37" s="77">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I37" s="41">
+        <v>13.893617021276597</v>
+      </c>
+      <c r="I37" s="78">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J37" t="s">
-        <v>246</v>
-      </c>
-      <c r="K37" s="74" t="s">
-        <v>249</v>
+        <v>13.06</v>
+      </c>
+      <c r="J37" s="74" t="s">
+        <v>245</v>
+      </c>
+      <c r="K37" s="79" t="s">
+        <v>248</v>
       </c>
       <c r="Q37" s="41"/>
     </row>
@@ -4420,30 +4465,19 @@
       <c r="B38" t="s">
         <v>73</v>
       </c>
-      <c r="E38" s="32">
-        <v>1</v>
-      </c>
-      <c r="F38" s="48"/>
-      <c r="G38" s="57"/>
-      <c r="H38" s="48">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I38" s="41">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J38" t="s">
-        <v>246</v>
-      </c>
-      <c r="K38" s="74" t="s">
-        <v>249</v>
-      </c>
+      <c r="C38" s="75"/>
+      <c r="E38" s="76"/>
+      <c r="F38" s="77"/>
+      <c r="G38" s="80"/>
+      <c r="H38" s="77"/>
+      <c r="I38" s="78"/>
+      <c r="J38" s="74"/>
+      <c r="K38" s="79"/>
       <c r="P38" s="41">
         <v>128.36584400000004</v>
       </c>
       <c r="Q38" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="S38" s="41"/>
     </row>
@@ -4454,26 +4488,14 @@
       <c r="B39" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="63"/>
-      <c r="E39" s="32">
-        <v>1</v>
-      </c>
-      <c r="F39" s="48"/>
-      <c r="G39" s="57"/>
-      <c r="H39" s="48">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I39" s="41">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J39" t="s">
-        <v>246</v>
-      </c>
-      <c r="K39" s="74" t="s">
-        <v>249</v>
-      </c>
+      <c r="C39" s="75"/>
+      <c r="E39" s="76"/>
+      <c r="F39" s="77"/>
+      <c r="G39" s="80"/>
+      <c r="H39" s="77"/>
+      <c r="I39" s="78"/>
+      <c r="J39" s="74"/>
+      <c r="K39" s="79"/>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="28" t="s">
@@ -4482,25 +4504,14 @@
       <c r="B40" t="s">
         <v>75</v>
       </c>
-      <c r="E40" s="32">
-        <v>1</v>
-      </c>
-      <c r="F40" s="48"/>
-      <c r="G40" s="57"/>
-      <c r="H40" s="48">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I40" s="41">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J40" t="s">
-        <v>246</v>
-      </c>
-      <c r="K40" s="74" t="s">
-        <v>249</v>
-      </c>
+      <c r="C40" s="75"/>
+      <c r="E40" s="76"/>
+      <c r="F40" s="77"/>
+      <c r="G40" s="80"/>
+      <c r="H40" s="77"/>
+      <c r="I40" s="78"/>
+      <c r="J40" s="74"/>
+      <c r="K40" s="79"/>
       <c r="Q40" s="41"/>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
@@ -4510,25 +4521,14 @@
       <c r="B41" t="s">
         <v>76</v>
       </c>
-      <c r="E41" s="32">
-        <v>1</v>
-      </c>
-      <c r="F41" s="48"/>
-      <c r="G41" s="57"/>
-      <c r="H41" s="48">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I41" s="41">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J41" t="s">
-        <v>246</v>
-      </c>
-      <c r="K41" s="74" t="s">
-        <v>249</v>
-      </c>
+      <c r="C41" s="75"/>
+      <c r="E41" s="76"/>
+      <c r="F41" s="77"/>
+      <c r="G41" s="80"/>
+      <c r="H41" s="77"/>
+      <c r="I41" s="78"/>
+      <c r="J41" s="74"/>
+      <c r="K41" s="79"/>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="28" t="s">
@@ -4562,10 +4562,10 @@
         <v>1.5</v>
       </c>
       <c r="J42" t="s">
-        <v>245</v>
-      </c>
-      <c r="K42" s="69" t="s">
-        <v>250</v>
+        <v>270</v>
+      </c>
+      <c r="K42" s="68" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="43" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4602,7 +4602,7 @@
         <v>49.03</v>
       </c>
       <c r="H44" s="48">
-        <f t="shared" ref="H44:H49" si="7">E44*F44</f>
+        <f t="shared" ref="H44:H49" si="8">E44*F44</f>
         <v>52.159574468085111</v>
       </c>
       <c r="I44" s="41">
@@ -4610,7 +4610,7 @@
         <v>49.03</v>
       </c>
       <c r="J44" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
@@ -4618,7 +4618,7 @@
         <v>227</v>
       </c>
       <c r="C45" s="29" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E45" s="32">
         <v>1</v>
@@ -4631,7 +4631,7 @@
         <v>1.4852000000000001</v>
       </c>
       <c r="H45" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.58</v>
       </c>
       <c r="I45" s="41">
@@ -4639,7 +4639,7 @@
         <v>1.4852000000000001</v>
       </c>
       <c r="J45" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
@@ -4647,7 +4647,7 @@
         <v>228</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E46" s="32">
         <v>1</v>
@@ -4660,7 +4660,7 @@
         <v>0.33839999999999998</v>
       </c>
       <c r="H46" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.36</v>
       </c>
       <c r="I46" s="41">
@@ -4668,7 +4668,7 @@
         <v>0.33839999999999998</v>
       </c>
       <c r="J46" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
@@ -4689,7 +4689,7 @@
         <v>9.99</v>
       </c>
       <c r="H47" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10.627659574468085</v>
       </c>
       <c r="I47" s="41">
@@ -4697,7 +4697,7 @@
         <v>9.99</v>
       </c>
       <c r="J47" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
@@ -4718,7 +4718,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="H48" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.1914893617021278</v>
       </c>
       <c r="I48" s="41">
@@ -4726,7 +4726,7 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="J48" t="s">
-        <v>245</v>
+        <v>270</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -4747,7 +4747,7 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="H49" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2340425531914894</v>
       </c>
       <c r="I49" s="41">
@@ -4755,7 +4755,7 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="J49" t="s">
-        <v>245</v>
+        <v>270</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -4775,15 +4775,15 @@
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E51">
         <f>SUM(E3:E49)</f>
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H51" s="48">
         <f>SUM(H3:H49)</f>
-        <v>95.68608936170213</v>
+        <v>109.57970638297871</v>
       </c>
       <c r="I51" s="41">
         <f>SUM(I3:I49)</f>
-        <v>89.944924</v>
+        <v>103.004924</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -4794,7 +4794,7 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -4802,10 +4802,10 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="C56" s="73" t="s">
-        <v>266</v>
+        <v>268</v>
+      </c>
+      <c r="C56" s="72" t="s">
+        <v>265</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1">
@@ -4815,22 +4815,30 @@
         <v>1.29</v>
       </c>
       <c r="J56" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C57" s="1"/>
+        <v>269</v>
+      </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="C58" s="1"/>
+      <c r="A58" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>274</v>
+      </c>
       <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
+      <c r="E58" s="1">
+        <v>10</v>
+      </c>
+      <c r="G58">
+        <v>4.16</v>
+      </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
@@ -4843,7 +4851,22 @@
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
     </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="C37:C41"/>
+    <mergeCell ref="E37:E41"/>
+    <mergeCell ref="H37:H41"/>
+    <mergeCell ref="I37:I41"/>
+    <mergeCell ref="J37:J41"/>
+    <mergeCell ref="K37:K41"/>
+    <mergeCell ref="G37:G41"/>
+    <mergeCell ref="F37:F41"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="C34" r:id="rId1" xr:uid="{6AF00EDC-69E7-4B88-A944-F8CEFBA4187A}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{D5B8ED5B-C8F4-49B1-B474-82D88E431403}"/>
@@ -4880,9 +4903,11 @@
     <hyperlink ref="C45" r:id="rId33" xr:uid="{9FFCAB6B-B425-4662-9851-FFC8B94CAE45}"/>
     <hyperlink ref="C46" r:id="rId34" xr:uid="{0F6E49AF-4BAA-49B1-87E6-98CA56E983C2}"/>
     <hyperlink ref="C56" r:id="rId35" xr:uid="{A9AEA7C2-91AB-4B6E-A63D-CE8D39625EB5}"/>
+    <hyperlink ref="C58" r:id="rId36" xr:uid="{E633E699-1ADE-4ACF-A106-60857CABBAE4}"/>
+    <hyperlink ref="C37" r:id="rId37" xr:uid="{F4A0B343-AD81-4925-8716-65AFC60B59B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId36"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId38"/>
 </worksheet>
 </file>
 

</xml_diff>